<commit_message>
edited the parts spreadsheet
</commit_message>
<xml_diff>
--- a/Project QUBO/eagleDesigns/Qubo New/Power Board/Robotics Powerboard Part List.xlsx
+++ b/Project QUBO/eagleDesigns/Qubo New/Power Board/Robotics Powerboard Part List.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anthonyostuni/Library/Mobile Documents/com~apple~CloudDocs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexj\Documents\Project Qubo\trunk\Project QUBO\eagleDesigns\Qubo New\Power Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A526B7-E18C-9C43-B42F-61EFABB8E6C1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A971691-6F56-4E96-A2DD-FDA27691340E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>Supplier</t>
   </si>
@@ -220,13 +220,25 @@
   </si>
   <si>
     <t>330 uF Capacitor</t>
+  </si>
+  <si>
+    <t>BCS-106-L-D-PE-BE</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/samtec-inc/BCS-106-L-D-PE-BE/SAM9053-ND/6628937</t>
+  </si>
+  <si>
+    <t>CONN RECEPT 2MM VERT AU 10POS</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/harwin-inc/M22-7131042/952-1354-5-ND/2264335</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -269,6 +281,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -291,7 +309,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -304,6 +322,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="40" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="40" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -619,13 +638,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="33.6640625" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" customWidth="1"/>
@@ -635,7 +654,7 @@
     <col min="7" max="7" width="64.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -655,7 +674,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -675,7 +694,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -695,7 +714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -715,7 +734,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -735,7 +754,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -755,7 +774,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>41</v>
       </c>
@@ -778,7 +797,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>59</v>
       </c>
@@ -798,7 +817,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -818,7 +837,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -838,7 +857,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -858,7 +877,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -878,7 +897,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -898,7 +917,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -918,7 +937,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -938,7 +957,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -958,7 +977,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -978,7 +997,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>63</v>
       </c>
@@ -996,6 +1015,28 @@
       </c>
       <c r="F19" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D20" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20">
+        <v>10</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D21" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1012,8 +1053,10 @@
     <hyperlink ref="F8" r:id="rId10" xr:uid="{B6D552BB-185A-7447-BD82-D43A0150EAA9}"/>
     <hyperlink ref="F10" r:id="rId11" xr:uid="{653EE4F2-BEA5-FA45-B161-E713FE4DF7BC}"/>
     <hyperlink ref="F9" r:id="rId12" xr:uid="{7674E973-257E-804F-ACA7-331423ADA78F}"/>
+    <hyperlink ref="F20" r:id="rId13" xr:uid="{C2AE9491-4374-4E10-9CAF-DB64302B404E}"/>
+    <hyperlink ref="F21" r:id="rId14" xr:uid="{83618CCC-2F42-44A1-BF70-BED045EA7DCB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>